<commit_message>
Generated AN160 TC2 scripts
</commit_message>
<xml_diff>
--- a/src/Pickles/MIL_pickles/Output/AN160_TestScript_Desktop_Admin_System_FR_NFR.xlsx
+++ b/src/Pickles/MIL_pickles/Output/AN160_TestScript_Desktop_Admin_System_FR_NFR.xlsx
@@ -8,8 +8,8 @@
   <x:sheets>
     <x:sheet name="TOC" sheetId="2" r:id="rId2"/>
     <x:sheet name="CUSTOMERPAYMENT" sheetId="3" r:id="rId3"/>
-    <x:sheet name="UPDATECLIENT" sheetId="4" r:id="rId4"/>
-    <x:sheet name="UPDATECLI(1)" sheetId="5" r:id="rId5"/>
+    <x:sheet name="DESKTOPLICENSING" sheetId="4" r:id="rId4"/>
+    <x:sheet name="UPDATECLIENT" sheetId="5" r:id="rId5"/>
     <x:sheet name="USERREGISTRATION" sheetId="6" r:id="rId6"/>
   </x:sheets>
   <x:definedNames/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="127">
   <x:si>
     <x:t>CustomerPayment</x:t>
   </x:si>
@@ -116,187 +116,190 @@
     <x:t>the invoice contains a statement regarding reverse tax</x:t>
   </x:si>
   <x:si>
+    <x:t>DesktopLicensing</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR, @FR027, @UR025, @Admin, @DesktopOnly</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RegisterUser</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR027-1, @UR025-1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>no licence exists for the current machine</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I start the desktop app</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the user registration form is displayed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I enter the registration details</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the desktop app starts</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ExpiredLicenceRestrictsAccess</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR027-2, @UR025-2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>a licence exists for the current machine</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the licence is expired</x:t>
+  </x:si>
+  <x:si>
+    <x:t>a message tells me to upgrade</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ExpiredLicenceRedirectsToUpgrade</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR027-3, @UR025-3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the upgrade trial licence web page is displayed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ManualUpgradeAvailable</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR027-4, @UR025-3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the licence is not expired</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the menu includes an option to upgrade</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ManualUpgradeLinksToStore</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR027-5, @UR025-3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I have started the desktop app</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I choose the menu option "Upgrade Licence"</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the choice of upgrade options is approriate to my country</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ValidLicence</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR027-6, @UR025-4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the desktop app opens</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DisplayLicence</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR027-7, @UR025-5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I open the About Box</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the licence key is displayed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the licence expiry date is displayed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the licensee is displayed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EnterNewLicenceKey</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR027-8, @UR025-6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I click Enter Key</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I enter a new valid key from the same CryptoLens product</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the key is accepted</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I restart the application</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the application restarts</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EnterNewLicenceKeyNewProduct</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR027-9, @UR025-6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I enter a new valid key prefixed with a new product id in the form "{product-id}:{licence-key}"</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PurchaseLicenseExtension</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR027-10, @UR025-7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I choose the Purchase Upgrade menu option</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I fill in my payment details</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I complete the purchase</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I restart the desktop app</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the license period is extended by the amount specified for the purchased product</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ConfigureTrialPeriod</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR027-11, @UR025-8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I configure the store app to generate a &lt;num1&gt; day(s) licence</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I register for a trial licence</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the licence expiry date can be seen in the application</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the expiry date is in &lt;num2&gt; day(s)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Examples</x:t>
+  </x:si>
+  <x:si>
+    <x:t>num1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>num2</x:t>
+  </x:si>
+  <x:si>
     <x:t>UpdateClient</x:t>
-  </x:si>
-  <x:si>
-    <x:t>@FR, @FR027, @UR025, @Admin, @DesktopOnly</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RegisterUser</x:t>
-  </x:si>
-  <x:si>
-    <x:t>@FR027-1, @UR025-1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>no licence exists for the current machine</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I start the desktop app</x:t>
-  </x:si>
-  <x:si>
-    <x:t>the user registration form is displayed</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I enter the registration details</x:t>
-  </x:si>
-  <x:si>
-    <x:t>the desktop app starts</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ExpiredLicenceRestrictsAccess</x:t>
-  </x:si>
-  <x:si>
-    <x:t>@FR027-2, @UR025-2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>a licence exists for the current machine</x:t>
-  </x:si>
-  <x:si>
-    <x:t>the licence is expired</x:t>
-  </x:si>
-  <x:si>
-    <x:t>a message tells me to upgrade</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ExpiredLicenceRedirectsToUpgrade</x:t>
-  </x:si>
-  <x:si>
-    <x:t>@FR027-3, @UR025-3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>the upgrade trial licence web page is displayed</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ManualUpgradeAvailable</x:t>
-  </x:si>
-  <x:si>
-    <x:t>@FR027-4, @UR025-3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>the licence is not expired</x:t>
-  </x:si>
-  <x:si>
-    <x:t>the menu includes an option to upgrade</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ManualUpgradeLinksToStore</x:t>
-  </x:si>
-  <x:si>
-    <x:t>@FR027-5, @UR025-3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I have started the desktop app</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I choose the menu option "Upgrade Licence"</x:t>
-  </x:si>
-  <x:si>
-    <x:t>the choice of upgrade options is approriate to my country</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ValidLicence</x:t>
-  </x:si>
-  <x:si>
-    <x:t>@FR027-6, @UR025-4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>the desktop app opens</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DisplayLicence</x:t>
-  </x:si>
-  <x:si>
-    <x:t>@FR027-7, @UR025-5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I open the About Box</x:t>
-  </x:si>
-  <x:si>
-    <x:t>the licence key is displayed</x:t>
-  </x:si>
-  <x:si>
-    <x:t>the licence expiry date is displayed</x:t>
-  </x:si>
-  <x:si>
-    <x:t>the licensee is displayed</x:t>
-  </x:si>
-  <x:si>
-    <x:t>EnterNewLicenceKey</x:t>
-  </x:si>
-  <x:si>
-    <x:t>@FR027-8, @UR025-6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I click Enter Key</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I enter a new valid key from the same CryptoLens product</x:t>
-  </x:si>
-  <x:si>
-    <x:t>the key is accepted</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I restart the application</x:t>
-  </x:si>
-  <x:si>
-    <x:t>the application restarts</x:t>
-  </x:si>
-  <x:si>
-    <x:t>EnterNewLicenceKeyNewProduct</x:t>
-  </x:si>
-  <x:si>
-    <x:t>@FR027-9, @UR025-6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I enter a new valid key prefixed with a new product id in the form "{product-id}:{licence-key}"</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PurchaseLicenseExtension</x:t>
-  </x:si>
-  <x:si>
-    <x:t>@FR027-10, @UR025-7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I choose the Purchase Upgrade menu option</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I fill in my payment details</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I complete the purchase</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I restart the desktop app</x:t>
-  </x:si>
-  <x:si>
-    <x:t>the license period is extended by the amount specified for the purchased product</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ConfigureTrialPeriod</x:t>
-  </x:si>
-  <x:si>
-    <x:t>@FR027-11, @UR025-8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I configure the store app to generate a &lt;num1&gt; day(s) licence</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I register for a trial licence</x:t>
-  </x:si>
-  <x:si>
-    <x:t>the licence expiry date can be seen in the application</x:t>
-  </x:si>
-  <x:si>
-    <x:t>the expiry date is in &lt;num2&gt; day(s)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Examples</x:t>
-  </x:si>
-  <x:si>
-    <x:t>num1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>num2</x:t>
   </x:si>
   <x:si>
     <x:t>@FR, @FR032, @Admin, @DesktopOnly</x:t>
@@ -852,7 +855,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:2">
       <x:c r="A1" s="1" t="s">
-        <x:v>125</x:v>
+        <x:v>126</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:2">
@@ -867,18 +870,18 @@
     </x:row>
     <x:row r="4" spans="1:2">
       <x:c r="B4" s="6" t="s">
-        <x:v>32</x:v>
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:2">
       <x:c r="B5" s="6" t="s">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
     <x:hyperlink ref="B2" location="'CUSTOMERPAYMENT'!A1" display="CustomerPayment"/>
-    <x:hyperlink ref="B3" location="'UPDATECLIENT'!A1" display="UpdateClient"/>
+    <x:hyperlink ref="B3" location="'DESKTOPLICENSING'!A1" display="DesktopLicensing"/>
     <x:hyperlink ref="B4" location="'UPDATECLIENT'!A1" display="UpdateClient"/>
     <x:hyperlink ref="B5" location="'USERREGISTRATION'!A1" display="UserRegistration"/>
   </x:hyperlinks>
@@ -1889,7 +1892,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
@@ -1897,13 +1900,13 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4"/>
     <x:row r="5" spans="1:4">
       <x:c r="B5" s="1" t="s">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
@@ -1911,7 +1914,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4"/>
@@ -1920,7 +1923,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
@@ -1928,7 +1931,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4">
@@ -1936,12 +1939,12 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>99</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:4">
       <x:c r="B12" s="1" t="s">
-        <x:v>99</x:v>
+        <x:v>100</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:4">
@@ -1949,7 +1952,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C13" s="2" t="s">
-        <x:v>100</x:v>
+        <x:v>101</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4"/>
@@ -1958,7 +1961,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>102</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:4">
@@ -1966,7 +1969,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:4">
@@ -1974,7 +1977,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>99</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:4">
@@ -1982,7 +1985,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>103</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:4">
@@ -1990,7 +1993,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>103</x:v>
+        <x:v>104</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:4">
@@ -1998,7 +2001,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>105</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -2023,7 +2026,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
@@ -2031,13 +2034,13 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4"/>
     <x:row r="5" spans="1:4">
       <x:c r="B5" s="1" t="s">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
@@ -2045,7 +2048,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
-        <x:v>108</x:v>
+        <x:v>109</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4"/>
@@ -2062,7 +2065,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>110</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4">
@@ -2075,7 +2078,7 @@
     </x:row>
     <x:row r="12" spans="1:4">
       <x:c r="B12" s="1" t="s">
-        <x:v>110</x:v>
+        <x:v>111</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:4">
@@ -2083,7 +2086,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C13" s="2" t="s">
-        <x:v>111</x:v>
+        <x:v>112</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4"/>
@@ -2100,7 +2103,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>110</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:4">
@@ -2108,7 +2111,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>112</x:v>
+        <x:v>113</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:4">
@@ -2116,7 +2119,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>113</x:v>
+        <x:v>114</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:4">
@@ -2124,7 +2127,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>115</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:4">
@@ -2132,7 +2135,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:4">
@@ -2140,12 +2143,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>117</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:4">
       <x:c r="B23" s="1" t="s">
-        <x:v>117</x:v>
+        <x:v>118</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:4">
@@ -2153,7 +2156,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C24" s="2" t="s">
-        <x:v>118</x:v>
+        <x:v>119</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:4"/>
@@ -2170,7 +2173,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D27" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>110</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:4">
@@ -2178,7 +2181,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D28" s="0" t="s">
-        <x:v>112</x:v>
+        <x:v>113</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:4">
@@ -2186,7 +2189,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D29" s="0" t="s">
-        <x:v>113</x:v>
+        <x:v>114</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:4">
@@ -2194,7 +2197,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D30" s="0" t="s">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:4">
@@ -2202,7 +2205,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D31" s="0" t="s">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:4">
@@ -2210,12 +2213,12 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D32" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>117</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:4">
       <x:c r="B34" s="1" t="s">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:4">
@@ -2223,7 +2226,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C35" s="2" t="s">
-        <x:v>121</x:v>
+        <x:v>122</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:4"/>
@@ -2240,7 +2243,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D38" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>110</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:4">
@@ -2248,7 +2251,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D39" s="0" t="s">
-        <x:v>112</x:v>
+        <x:v>113</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:4">
@@ -2256,7 +2259,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D40" s="0" t="s">
-        <x:v>113</x:v>
+        <x:v>114</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:4">
@@ -2264,7 +2267,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D41" s="0" t="s">
-        <x:v>122</x:v>
+        <x:v>123</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:4">
@@ -2272,7 +2275,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D42" s="0" t="s">
-        <x:v>123</x:v>
+        <x:v>124</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:4">
@@ -2280,7 +2283,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D43" s="0" t="s">
-        <x:v>124</x:v>
+        <x:v>125</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>